<commit_message>
Results from July 28, 2020 04:21:04 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-28.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-28.xlsx
@@ -609,23 +609,23 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>220483</t>
+          <t>220907</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18872</t>
+          <t>18878</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>34116</v>
+        <v>34141</v>
       </c>
       <c r="F4" t="n">
-        <v>5261</v>
+        <v>5263</v>
       </c>
       <c r="G4" t="n">
         <v>29.91</v>
@@ -640,10 +640,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>114053</v>
+        <v>114142</v>
       </c>
       <c r="L4" t="n">
-        <v>17283</v>
+        <v>17290</v>
       </c>
       <c r="M4" t="n">
         <v>2049418</v>
@@ -791,21 +791,21 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>38409</t>
+          <t>38855</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>281</t>
+          <t>286</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>945</t>
+          <t>953</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -817,7 +817,7 @@
         <v>2.5</v>
       </c>
       <c r="H8" t="n">
-        <v>1.78</v>
+        <v>1.75</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -882,22 +882,22 @@
         <v>44040</v>
       </c>
       <c r="C10" t="n">
-        <v>39447</v>
+        <v>40181</v>
       </c>
       <c r="D10" t="n">
-        <v>408</v>
+        <v>428</v>
       </c>
       <c r="E10" t="n">
-        <v>8264</v>
+        <v>8424</v>
       </c>
       <c r="F10" t="n">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G10" t="n">
-        <v>24.39</v>
+        <v>24.35</v>
       </c>
       <c r="H10" t="n">
-        <v>25.98</v>
+        <v>25.88</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -906,10 +906,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>33884</v>
+        <v>34593</v>
       </c>
       <c r="L10" t="n">
-        <v>408</v>
+        <v>425</v>
       </c>
       <c r="M10" t="n">
         <v>460970</v>
@@ -1028,16 +1028,16 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C13" t="n">
-        <v>19502</v>
+        <v>19791</v>
       </c>
       <c r="D13" t="n">
-        <v>619</v>
+        <v>626</v>
       </c>
       <c r="E13" t="n">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
@@ -1212,25 +1212,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C17" t="n">
-        <v>176028</v>
+        <v>178642</v>
       </c>
       <c r="D17" t="n">
-        <v>4375</v>
+        <v>4426</v>
       </c>
       <c r="E17" t="n">
-        <v>4727</v>
+        <v>4774</v>
       </c>
       <c r="F17" t="n">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="G17" t="n">
-        <v>4.61</v>
+        <v>4.62</v>
       </c>
       <c r="H17" t="n">
-        <v>10.73</v>
+        <v>10.67</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1239,10 +1239,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>102449</v>
+        <v>103302</v>
       </c>
       <c r="L17" t="n">
-        <v>4083</v>
+        <v>4133</v>
       </c>
       <c r="M17" t="n">
         <v>823987</v>
@@ -1314,19 +1314,19 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C19" t="n">
-        <v>52957</v>
+        <v>54299</v>
       </c>
       <c r="D19" t="n">
-        <v>1501</v>
+        <v>1543</v>
       </c>
       <c r="E19" t="n">
-        <v>23006</v>
+        <v>23585</v>
       </c>
       <c r="F19" t="n">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="G19" t="n">
         <v>43.44</v>
@@ -1412,22 +1412,22 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C21" t="n">
-        <v>105228</v>
+        <v>106331</v>
       </c>
       <c r="D21" t="n">
-        <v>7122</v>
+        <v>7146</v>
       </c>
       <c r="E21" t="n">
-        <v>14751</v>
+        <v>15052</v>
       </c>
       <c r="F21" t="n">
         <v>1484</v>
       </c>
       <c r="G21" t="n">
-        <v>29.77</v>
+        <v>29.82</v>
       </c>
       <c r="H21" t="n">
         <v>21.22</v>
@@ -1439,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>49557</v>
+        <v>50476</v>
       </c>
       <c r="L21" t="n">
         <v>6992</v>
@@ -1510,20 +1510,20 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C23" t="n">
-        <v>3381</v>
+        <v>3475</v>
       </c>
       <c r="D23" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E23" t="n">
         <v>20</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>0.59</v>
+        <v>0.58</v>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="b">
@@ -1604,22 +1604,22 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C25" t="n">
-        <v>46994</v>
+        <v>47089</v>
       </c>
       <c r="D25" t="n">
-        <v>3536</v>
+        <v>3541</v>
       </c>
       <c r="E25" t="n">
-        <v>6436</v>
+        <v>6443</v>
       </c>
       <c r="F25" t="n">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="G25" t="n">
-        <v>13.7</v>
+        <v>13.68</v>
       </c>
       <c r="H25" t="n">
         <v>18.47</v>
@@ -1702,25 +1702,25 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C27" t="n">
-        <v>44565</v>
+        <v>45314</v>
       </c>
       <c r="D27" t="n">
-        <v>1799</v>
+        <v>1807</v>
       </c>
       <c r="E27" t="n">
-        <v>2108</v>
+        <v>2130</v>
       </c>
       <c r="F27" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G27" t="n">
-        <v>6.09</v>
+        <v>6.07</v>
       </c>
       <c r="H27" t="n">
-        <v>6.85</v>
+        <v>6.93</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
@@ -1729,10 +1729,10 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>34627</v>
+        <v>35069</v>
       </c>
       <c r="L27" t="n">
-        <v>1737</v>
+        <v>1745</v>
       </c>
       <c r="M27" t="n">
         <v>227938</v>
@@ -1753,25 +1753,25 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C28" t="n">
-        <v>24899</v>
+        <v>25157</v>
       </c>
       <c r="D28" t="n">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E28" t="n">
-        <v>1511</v>
+        <v>1540</v>
       </c>
       <c r="F28" t="n">
         <v>24</v>
       </c>
       <c r="G28" t="n">
-        <v>7.84</v>
+        <v>7.85</v>
       </c>
       <c r="H28" t="n">
-        <v>7.92</v>
+        <v>7.87</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
@@ -1780,10 +1780,10 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>19282</v>
+        <v>19625</v>
       </c>
       <c r="L28" t="n">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="M28" t="n">
         <v>90860</v>
@@ -1804,25 +1804,25 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C29" t="n">
-        <v>78419</v>
+        <v>79090</v>
       </c>
       <c r="D29" t="n">
-        <v>6075</v>
+        <v>6091</v>
       </c>
       <c r="E29" t="n">
-        <v>21927</v>
+        <v>22020</v>
       </c>
       <c r="F29" t="n">
-        <v>2422</v>
+        <v>2426</v>
       </c>
       <c r="G29" t="n">
-        <v>27.96</v>
+        <v>27.84</v>
       </c>
       <c r="H29" t="n">
-        <v>39.87</v>
+        <v>39.83</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -1854,10 +1854,10 @@
         <v>44034</v>
       </c>
       <c r="C30" t="n">
-        <v>109917</v>
+        <v>111038</v>
       </c>
       <c r="D30" t="n">
-        <v>3674</v>
+        <v>3700</v>
       </c>
       <c r="E30" t="n">
         <v>36693</v>
@@ -1902,25 +1902,25 @@
         </is>
       </c>
       <c r="B31" s="3" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C31" t="n">
-        <v>460550</v>
+        <v>466550</v>
       </c>
       <c r="D31" t="n">
-        <v>8445</v>
+        <v>8518</v>
       </c>
       <c r="E31" t="n">
-        <v>12741</v>
+        <v>12866</v>
       </c>
       <c r="F31" t="n">
         <v>701</v>
       </c>
       <c r="G31" t="n">
-        <v>4.32</v>
+        <v>4.3</v>
       </c>
       <c r="H31" t="n">
-        <v>8.51</v>
+        <v>8.49</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -1929,10 +1929,10 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>295103</v>
+        <v>298953</v>
       </c>
       <c r="L31" t="n">
-        <v>8238</v>
+        <v>8261</v>
       </c>
       <c r="M31" t="n">
         <v>2267875</v>
@@ -1953,25 +1953,25 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C32" t="n">
-        <v>62907</v>
+        <v>63678</v>
       </c>
       <c r="D32" t="n">
-        <v>2709</v>
+        <v>2725</v>
       </c>
       <c r="E32" t="n">
-        <v>7242</v>
+        <v>7305</v>
       </c>
       <c r="F32" t="n">
         <v>383</v>
       </c>
       <c r="G32" t="n">
-        <v>11.51</v>
+        <v>11.47</v>
       </c>
       <c r="H32" t="n">
-        <v>14.14</v>
+        <v>14.06</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -2000,22 +2000,22 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C33" t="n">
-        <v>1638</v>
+        <v>1699</v>
       </c>
       <c r="D33" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E33" t="n">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>4.78</v>
+        <v>4.94</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2027,10 +2027,10 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>1506</v>
+        <v>1560</v>
       </c>
       <c r="L33" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M33" t="n">
         <v>24129</v>
@@ -2051,25 +2051,25 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C34" t="n">
-        <v>49417</v>
+        <v>50179</v>
       </c>
       <c r="D34" t="n">
-        <v>893</v>
+        <v>906</v>
       </c>
       <c r="E34" t="n">
-        <v>7632</v>
+        <v>7716</v>
       </c>
       <c r="F34" t="n">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G34" t="n">
-        <v>17.12</v>
+        <v>17.01</v>
       </c>
       <c r="H34" t="n">
-        <v>22.92</v>
+        <v>22.97</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
@@ -2078,10 +2078,10 @@
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>44574</v>
+        <v>45352</v>
       </c>
       <c r="L34" t="n">
-        <v>877</v>
+        <v>888</v>
       </c>
       <c r="M34" t="n">
         <v>368744</v>
@@ -2102,25 +2102,25 @@
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C35" t="n">
-        <v>170843</v>
+        <v>175052</v>
       </c>
       <c r="D35" t="n">
-        <v>3509</v>
+        <v>3563</v>
       </c>
       <c r="E35" t="n">
-        <v>43914</v>
+        <v>44977</v>
       </c>
       <c r="F35" t="n">
-        <v>1598</v>
+        <v>1617</v>
       </c>
       <c r="G35" t="n">
-        <v>25.7</v>
+        <v>25.69</v>
       </c>
       <c r="H35" t="n">
-        <v>45.54</v>
+        <v>45.38</v>
       </c>
       <c r="I35" t="b">
         <v>1</v>
@@ -2200,16 +2200,16 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C37" t="n">
-        <v>6441</v>
+        <v>6500</v>
       </c>
       <c r="D37" t="n">
         <v>409</v>
       </c>
       <c r="E37" t="n">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="F37" t="n">
         <v>9</v>
@@ -2227,7 +2227,7 @@
         <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>5595</v>
+        <v>5630</v>
       </c>
       <c r="L37" t="n">
         <v>406</v>
@@ -2379,19 +2379,19 @@
         <v>44040</v>
       </c>
       <c r="C41" t="n">
-        <v>42738</v>
+        <v>42789</v>
       </c>
       <c r="D41" t="n">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="E41" t="n">
-        <v>3394</v>
+        <v>3404</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
       </c>
       <c r="G41" t="n">
-        <v>7.94</v>
+        <v>7.96</v>
       </c>
       <c r="H41" t="n">
         <v>4.53</v>
@@ -2423,25 +2423,25 @@
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C42" t="n">
-        <v>114338</v>
+        <v>116087</v>
       </c>
       <c r="D42" t="n">
-        <v>1790</v>
+        <v>1820</v>
       </c>
       <c r="E42" t="n">
-        <v>19338</v>
+        <v>19790</v>
       </c>
       <c r="F42" t="n">
-        <v>560</v>
+        <v>569</v>
       </c>
       <c r="G42" t="n">
-        <v>24.01</v>
+        <v>24.04</v>
       </c>
       <c r="H42" t="n">
-        <v>32.43</v>
+        <v>32.38</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
@@ -2450,10 +2450,10 @@
         <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>80533</v>
+        <v>82329</v>
       </c>
       <c r="L42" t="n">
-        <v>1727</v>
+        <v>1757</v>
       </c>
       <c r="M42" t="n">
         <v>2179622</v>
@@ -2474,25 +2474,25 @@
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C43" t="n">
-        <v>172655</v>
+        <v>173731</v>
       </c>
       <c r="D43" t="n">
-        <v>7416</v>
+        <v>7446</v>
       </c>
       <c r="E43" t="n">
-        <v>28718</v>
+        <v>28884</v>
       </c>
       <c r="F43" t="n">
-        <v>2036</v>
+        <v>2043</v>
       </c>
       <c r="G43" t="n">
         <v>16.63</v>
       </c>
       <c r="H43" t="n">
-        <v>27.45</v>
+        <v>27.44</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
@@ -2521,25 +2521,25 @@
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C44" t="n">
-        <v>18694</v>
+        <v>19222</v>
       </c>
       <c r="D44" t="n">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E44" t="n">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F44" t="n">
         <v>3</v>
       </c>
       <c r="G44" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="H44" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
@@ -2567,21 +2567,39 @@
           <t>Ohio</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+      <c r="B45" s="2" t="n">
+        <v>44040</v>
+      </c>
+      <c r="C45" t="n">
+        <v>86497</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3382</v>
+      </c>
+      <c r="E45" t="n">
+        <v>21925</v>
+      </c>
+      <c r="F45" t="n">
+        <v>652</v>
+      </c>
+      <c r="G45" t="n">
+        <v>29.34</v>
+      </c>
+      <c r="H45" t="n">
+        <v>19.63</v>
+      </c>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="b">
-        <v>0</v>
-      </c>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K45" t="n">
+        <v>74731</v>
+      </c>
+      <c r="L45" t="n">
+        <v>3322</v>
+      </c>
       <c r="M45" t="n">
         <v>1438271</v>
       </c>
@@ -2590,7 +2608,7 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>An error occurred. ... JSONDecodeError('Expecting value: line 1 column 1 (char 0)')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -2601,25 +2619,25 @@
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C46" t="n">
-        <v>51803</v>
+        <v>52281</v>
       </c>
       <c r="D46" t="n">
-        <v>1576</v>
+        <v>1580</v>
       </c>
       <c r="E46" t="n">
-        <v>10638</v>
+        <v>10776</v>
       </c>
       <c r="F46" t="n">
         <v>149</v>
       </c>
       <c r="G46" t="n">
-        <v>20.54</v>
+        <v>20.61</v>
       </c>
       <c r="H46" t="n">
-        <v>9.449999999999999</v>
+        <v>9.43</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
@@ -2648,19 +2666,19 @@
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C47" t="n">
-        <v>115926</v>
+        <v>116182</v>
       </c>
       <c r="D47" t="n">
-        <v>8536</v>
+        <v>8551</v>
       </c>
       <c r="E47" t="n">
-        <v>10845</v>
+        <v>10870</v>
       </c>
       <c r="F47" t="n">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="G47" t="n">
         <v>9.359999999999999</v>
@@ -2695,25 +2713,25 @@
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C48" t="n">
-        <v>18261</v>
+        <v>18485</v>
       </c>
       <c r="D48" t="n">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E48" t="n">
-        <v>5149</v>
+        <v>5198</v>
       </c>
       <c r="F48" t="n">
         <v>148</v>
       </c>
       <c r="G48" t="n">
-        <v>30.44</v>
+        <v>30.29</v>
       </c>
       <c r="H48" t="n">
-        <v>39.05</v>
+        <v>38.85</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
@@ -2722,10 +2740,10 @@
         <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>16918</v>
+        <v>17161</v>
       </c>
       <c r="L48" t="n">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="M48" t="n">
         <v>252321</v>
@@ -2746,25 +2764,25 @@
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C49" t="n">
-        <v>43045</v>
+        <v>44819</v>
       </c>
       <c r="D49" t="n">
-        <v>1201</v>
+        <v>1213</v>
       </c>
       <c r="E49" t="n">
-        <v>9264</v>
+        <v>9479</v>
       </c>
       <c r="F49" t="n">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="G49" t="n">
-        <v>28.41</v>
+        <v>27.96</v>
       </c>
       <c r="H49" t="n">
-        <v>34.17</v>
+        <v>34.39</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
@@ -2773,10 +2791,10 @@
         <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>32609</v>
+        <v>33899</v>
       </c>
       <c r="L49" t="n">
-        <v>1156</v>
+        <v>1169</v>
       </c>
       <c r="M49" t="n">
         <v>704896</v>
@@ -2797,17 +2815,17 @@
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>44038</v>
+        <v>44039</v>
       </c>
       <c r="C50" t="n">
-        <v>412344</v>
+        <v>412878</v>
       </c>
       <c r="D50" t="n">
-        <v>25117</v>
+        <v>25126</v>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="n">
-        <v>6354</v>
+        <v>6356</v>
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
@@ -2821,7 +2839,7 @@
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="n">
-        <v>23614</v>
+        <v>23623</v>
       </c>
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr"/>
@@ -2838,25 +2856,25 @@
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>44036</v>
+        <v>44040</v>
       </c>
       <c r="C51" t="n">
-        <v>78607</v>
+        <v>84109</v>
       </c>
       <c r="D51" t="n">
-        <v>1385</v>
+        <v>1565</v>
       </c>
       <c r="E51" t="n">
-        <v>26288</v>
+        <v>28332</v>
       </c>
       <c r="F51" t="n">
-        <v>573</v>
+        <v>642</v>
       </c>
       <c r="G51" t="n">
-        <v>37.88</v>
+        <v>38.21</v>
       </c>
       <c r="H51" t="n">
-        <v>43.74</v>
+        <v>43.41</v>
       </c>
       <c r="I51" t="b">
         <v>0</v>
@@ -2865,10 +2883,10 @@
         <v>1</v>
       </c>
       <c r="K51" t="n">
-        <v>69406</v>
+        <v>74148</v>
       </c>
       <c r="L51" t="n">
-        <v>1310</v>
+        <v>1479</v>
       </c>
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr"/>

</xml_diff>

<commit_message>
Results from July 28, 2020 10:32:58 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-28.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-28.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,13 +558,13 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C3" t="n">
-        <v>36438</v>
+        <v>37984</v>
       </c>
       <c r="D3" t="n">
-        <v>323</v>
+        <v>335</v>
       </c>
       <c r="E3" t="n">
         <v>464</v>
@@ -733,7 +733,7 @@
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>An error occurred. ... KeyError('Date_Uploaded.Data as of')</t>
         </is>
       </c>
     </row>
@@ -744,25 +744,25 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C7" t="n">
-        <v>96489</v>
+        <v>99044</v>
       </c>
       <c r="D7" t="n">
-        <v>978</v>
+        <v>999</v>
       </c>
       <c r="E7" t="n">
-        <v>18408</v>
+        <v>18749</v>
       </c>
       <c r="F7" t="n">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="G7" t="n">
-        <v>19.08</v>
+        <v>18.93</v>
       </c>
       <c r="H7" t="n">
-        <v>34.46</v>
+        <v>34.33</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -930,25 +930,25 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C11" t="n">
-        <v>27507</v>
+        <v>28005</v>
       </c>
       <c r="D11" t="n">
-        <v>533</v>
+        <v>547</v>
       </c>
       <c r="E11" t="n">
-        <v>1012</v>
+        <v>1034</v>
       </c>
       <c r="F11" t="n">
         <v>20</v>
       </c>
       <c r="G11" t="n">
-        <v>4.71</v>
+        <v>4.73</v>
       </c>
       <c r="H11" t="n">
-        <v>3.86</v>
+        <v>3.77</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -957,10 +957,10 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>21477</v>
+        <v>21845</v>
       </c>
       <c r="L11" t="n">
-        <v>518</v>
+        <v>531</v>
       </c>
       <c r="M11" t="n">
         <v>166412</v>
@@ -2149,25 +2149,25 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="C36" t="n">
-        <v>53321</v>
+        <v>54205</v>
       </c>
       <c r="D36" t="n">
-        <v>1518</v>
+        <v>1548</v>
       </c>
       <c r="E36" t="n">
-        <v>1930</v>
+        <v>1984</v>
       </c>
       <c r="F36" t="n">
         <v>49</v>
       </c>
       <c r="G36" t="n">
-        <v>5.44</v>
+        <v>5.52</v>
       </c>
       <c r="H36" t="n">
-        <v>3.31</v>
+        <v>3.26</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -2176,10 +2176,10 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>35454</v>
+        <v>35958</v>
       </c>
       <c r="L36" t="n">
-        <v>1479</v>
+        <v>1505</v>
       </c>
       <c r="M36" t="n">
         <v>269854</v>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
+          <t>An error occurred. ... WebDriverException('unknown error: session deleted because of page crash\nfrom unknown error: cannot determine loading status\nfrom tab crashed\n  (Session info: headless chrome=83.0.4103.116)', None, None)</t>
         </is>
       </c>
     </row>
@@ -2376,22 +2376,22 @@
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C41" t="n">
-        <v>42789</v>
+        <v>42928</v>
       </c>
       <c r="D41" t="n">
         <v>839</v>
       </c>
       <c r="E41" t="n">
-        <v>3404</v>
+        <v>3407</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
       </c>
       <c r="G41" t="n">
-        <v>7.96</v>
+        <v>7.94</v>
       </c>
       <c r="H41" t="n">
         <v>4.53</v>
@@ -2567,39 +2567,21 @@
           <t>Ohio</t>
         </is>
       </c>
-      <c r="B45" s="2" t="n">
-        <v>44040</v>
-      </c>
-      <c r="C45" t="n">
-        <v>86497</v>
-      </c>
-      <c r="D45" t="n">
-        <v>3382</v>
-      </c>
-      <c r="E45" t="n">
-        <v>21925</v>
-      </c>
-      <c r="F45" t="n">
-        <v>652</v>
-      </c>
-      <c r="G45" t="n">
-        <v>29.34</v>
-      </c>
-      <c r="H45" t="n">
-        <v>19.63</v>
-      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K45" t="n">
-        <v>74731</v>
-      </c>
-      <c r="L45" t="n">
-        <v>3322</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
       <c r="M45" t="n">
         <v>1438271</v>
       </c>
@@ -2608,7 +2590,7 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'body'")</t>
         </is>
       </c>
     </row>
@@ -2814,23 +2796,13 @@
           <t>NewYork</t>
         </is>
       </c>
-      <c r="B50" s="2" t="n">
-        <v>44039</v>
-      </c>
-      <c r="C50" t="n">
-        <v>412878</v>
-      </c>
-      <c r="D50" t="n">
-        <v>25126</v>
-      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" t="n">
-        <v>6356</v>
-      </c>
+      <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
-      <c r="H50" t="n">
-        <v>26.91</v>
-      </c>
+      <c r="H50" t="inlineStr"/>
       <c r="I50" t="b">
         <v>0</v>
       </c>
@@ -2838,59 +2810,131 @@
         <v>0</v>
       </c>
       <c r="K50" t="inlineStr"/>
-      <c r="L50" t="n">
-        <v>23623</v>
-      </c>
+      <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... ConnectionRefusedError(111, 'Connection refused')</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>Wyoming</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="n">
+        <v>5540</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>An error occurred. ... JSONDecodeError('Expecting value: line 1 column 1 (char 0)')</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>SouthDakota</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="n">
+        <v>44040</v>
+      </c>
+      <c r="C52" t="n">
+        <v>8492</v>
+      </c>
+      <c r="D52" t="n">
+        <v>123</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1008</v>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>11.87</v>
+      </c>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>8492</v>
+      </c>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
           <t>SouthCarolina</t>
         </is>
       </c>
-      <c r="B51" s="2" t="n">
-        <v>44040</v>
-      </c>
-      <c r="C51" t="n">
+      <c r="B53" s="2" t="n">
+        <v>44040</v>
+      </c>
+      <c r="C53" t="n">
         <v>84109</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D53" t="n">
         <v>1565</v>
       </c>
-      <c r="E51" t="n">
+      <c r="E53" t="n">
         <v>28332</v>
       </c>
-      <c r="F51" t="n">
+      <c r="F53" t="n">
         <v>642</v>
       </c>
-      <c r="G51" t="n">
+      <c r="G53" t="n">
         <v>38.21</v>
       </c>
-      <c r="H51" t="n">
+      <c r="H53" t="n">
         <v>43.41</v>
       </c>
-      <c r="I51" t="b">
-        <v>0</v>
-      </c>
-      <c r="J51" t="b">
-        <v>1</v>
-      </c>
-      <c r="K51" t="n">
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+      <c r="J53" t="b">
+        <v>1</v>
+      </c>
+      <c r="K53" t="n">
         <v>74148</v>
       </c>
-      <c r="L51" t="n">
+      <c r="L53" t="n">
         <v>1479</v>
       </c>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr">
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr">
         <is>
           <t>Success!</t>
         </is>

</xml_diff>